<commit_message>
use iiif image api
</commit_message>
<xml_diff>
--- a/src/data/main.xlsx
+++ b/src/data/main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nakamurasatoru/git/d_aozora/letter/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91950716-0B36-2D4E-B21B-BA9118475510}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BE94A5-C670-CC4E-A8A6-5DC8C9232CA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="item" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -152,6 +152,14 @@
   <si>
     <t>https://tei-eaj.github.io/letter/iiif/collection/top.json</t>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://05r4t6462c.execute-api.us-east-1.amazonaws.com/latest/iiif/2/tei-eaj%2Fletter2/info.json</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://05r4t6462c.execute-api.us-east-1.amazonaws.com/latest/iiif/2/tei-eaj%2Fletter1/info.json</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -6882,8 +6890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B8C668-124E-AE46-ABF1-E3A5FA928B92}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -6917,9 +6925,8 @@
       <c r="A2" s="7">
         <v>8205</v>
       </c>
-      <c r="B2" s="6" t="str">
-        <f>"https://tei-eaj.github.io/letter/files/original/letter1.jpg"</f>
-        <v>https://tei-eaj.github.io/letter/files/original/letter1.jpg</v>
+      <c r="B2" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="6" t="str">
         <f>"https://tei-eaj.github.io/letter/files/original/letter1.jpg"</f>
@@ -6936,9 +6943,8 @@
       <c r="A3" s="7">
         <v>8205</v>
       </c>
-      <c r="B3" s="6" t="str">
-        <f>"https://tei-eaj.github.io/letter/files/original/letter2.jpg"</f>
-        <v>https://tei-eaj.github.io/letter/files/original/letter2.jpg</v>
+      <c r="B3" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="C3" s="6" t="str">
         <f>"https://tei-eaj.github.io/letter/files/original/letter2.jpg"</f>
@@ -6954,10 +6960,10 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://iiif.dl.itc.u-tokyo.ac.jp/iiif/tmp/toyo/suikei/Etsunan.tif/info.json" xr:uid="{36672D0A-B1CC-9744-AD9C-1E5275D8D1E4}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://iiif.dl.itc.u-tokyo.ac.jp/iiif/tmp/toyo/suikei/Etsunan.tif/info.json" xr:uid="{4E87B2FD-D422-3A45-80D2-C85452019A3C}"/>
-    <hyperlink ref="C2" r:id="rId3" display="https://iiif.dl.itc.u-tokyo.ac.jp/iiif/tmp/toyo/suikei/Etsunan.tif/info.json" xr:uid="{B3F96469-F063-C844-85C0-ACB4D787BD58}"/>
-    <hyperlink ref="C3" r:id="rId4" display="https://iiif.dl.itc.u-tokyo.ac.jp/iiif/tmp/toyo/suikei/Etsunan.tif/info.json" xr:uid="{5A7B9F79-2B52-8B48-8043-5ADCCC561477}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{36672D0A-B1CC-9744-AD9C-1E5275D8D1E4}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{6F67C072-D5BB-D545-82F7-C895775B06BD}"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://iiif.dl.itc.u-tokyo.ac.jp/iiif/tmp/toyo/suikei/Etsunan.tif/info.json" xr:uid="{5A7B9F79-2B52-8B48-8043-5ADCCC561477}"/>
+    <hyperlink ref="C2" r:id="rId4" display="https://iiif.dl.itc.u-tokyo.ac.jp/iiif/tmp/toyo/suikei/Etsunan.tif/info.json" xr:uid="{B3F96469-F063-C844-85C0-ACB4D787BD58}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6999,8 +7005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59CAB8B-6DA1-3A44-B198-2178D3D061BB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>

</xml_diff>